<commit_message>
add Load excel and log
</commit_message>
<xml_diff>
--- a/03 scripts/all columns.xlsx
+++ b/03 scripts/all columns.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="254">
   <si>
     <t xml:space="preserve">column name</t>
   </si>
@@ -493,9 +493,6 @@
   </si>
   <si>
     <t xml:space="preserve">Drop the 3rd cat?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w</t>
   </si>
   <si>
     <t xml:space="preserve">LabelEncoder</t>
@@ -898,13 +895,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0121457489879"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.51821862348178"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0445344129555"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2754,19 +2751,19 @@
   <dimension ref="A1:L123"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.412955465587"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3603238866397"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3000,9 +2997,6 @@
       <c r="D11" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -3041,7 +3035,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,13 +3052,13 @@
         <v>15</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>8</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>1</v>
@@ -3093,7 +3087,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>1</v>
@@ -3116,13 +3110,13 @@
         <v>15</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>1</v>
@@ -3151,7 +3145,7 @@
         <v>6</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>1</v>
@@ -3348,7 +3342,7 @@
         <v>18</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3413,7 +3407,7 @@
         <v>7</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4716,13 +4710,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.06882591093117"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.98380566801619"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.17813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.03643724696356"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4765,7 +4759,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -4793,7 +4787,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -4807,7 +4801,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -4821,7 +4815,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -4835,7 +4829,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2905</v>
@@ -4849,7 +4843,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -4863,7 +4857,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2905</v>
@@ -4899,13 +4893,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3522267206478"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4948,7 +4942,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -4962,7 +4956,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -4976,7 +4970,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -4988,7 +4982,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>8</v>
@@ -5018,13 +5012,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.74089068825911"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.74898785425101"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5067,7 +5061,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -5095,7 +5089,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -5109,7 +5103,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>26071</v>
@@ -5123,7 +5117,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>26087</v>
@@ -5137,7 +5131,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -5149,7 +5143,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>9</v>
@@ -5157,7 +5151,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -5171,7 +5165,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -5207,13 +5201,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2914979757085"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.06882591093117"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.98380566801619"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.17813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.03643724696356"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5306,13 +5300,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8461538461538"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1457489878543"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5369,7 +5363,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -5383,7 +5377,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -5395,7 +5389,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>4</v>
@@ -5403,7 +5397,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -5415,7 +5409,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>4</v>
@@ -5423,7 +5417,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -5437,7 +5431,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0</v>
@@ -5451,7 +5445,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>105553</v>
@@ -5465,7 +5459,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>633653</v>
@@ -5479,7 +5473,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1124488</v>
@@ -5493,7 +5487,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -5507,7 +5501,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>13</v>
@@ -5521,7 +5515,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>257669</v>
@@ -5535,7 +5529,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>591780</v>
@@ -5549,7 +5543,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -5563,7 +5557,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -5575,7 +5569,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>15</v>
@@ -5583,7 +5577,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -5633,13 +5627,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8785425101215"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0890688259109"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.60323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.07692307692308"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1336032388664"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5682,7 +5676,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -5710,7 +5704,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -5724,7 +5718,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -5738,7 +5732,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -5752,7 +5746,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>749816</v>
@@ -5766,7 +5760,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -5780,7 +5774,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>749816</v>
@@ -5794,7 +5788,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>749816</v>
@@ -5808,7 +5802,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>305236</v>
@@ -5822,7 +5816,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>767988</v>
@@ -5836,7 +5830,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -5850,7 +5844,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -5864,7 +5858,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
@@ -5878,7 +5872,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -5892,7 +5886,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>749816</v>
@@ -5906,7 +5900,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -5920,7 +5914,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>749816</v>
@@ -5934,7 +5928,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>749816</v>
@@ -5948,7 +5942,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>305236</v>
@@ -5962,7 +5956,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>0</v>
@@ -5974,7 +5968,7 @@
         <v>15</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>7</v>
@@ -5982,7 +5976,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -5996,7 +5990,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -6032,13 +6026,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.0364372469636"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6518218623482"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.60323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.080971659919"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1336032388664"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6081,7 +6075,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -6121,7 +6115,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>4</v>
@@ -6143,7 +6137,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -6171,7 +6165,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>895844</v>
@@ -6233,7 +6227,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -6253,7 +6247,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -6267,7 +6261,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>895844</v>
@@ -6281,7 +6275,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1664263</v>
@@ -6295,7 +6289,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1664263</v>
@@ -6309,7 +6303,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0</v>
@@ -6321,7 +6315,7 @@
         <v>15</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>25</v>
@@ -6329,7 +6323,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -6341,7 +6335,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>4</v>
@@ -6349,7 +6343,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -6363,7 +6357,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -6375,7 +6369,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>4</v>
@@ -6383,7 +6377,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0</v>
@@ -6395,7 +6389,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>9</v>
@@ -6423,7 +6417,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>0</v>
@@ -6435,7 +6429,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>4</v>
@@ -6443,7 +6437,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -6455,7 +6449,7 @@
         <v>15</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>28</v>
@@ -6463,7 +6457,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>0</v>
@@ -6475,7 +6469,7 @@
         <v>15</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>5</v>
@@ -6483,7 +6477,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -6495,7 +6489,7 @@
         <v>15</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>3</v>
@@ -6503,7 +6497,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -6515,7 +6509,7 @@
         <v>15</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>8</v>
@@ -6523,7 +6517,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
@@ -6537,7 +6531,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>0</v>
@@ -6549,7 +6543,7 @@
         <v>15</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>11</v>
@@ -6557,7 +6551,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>372230</v>
@@ -6571,7 +6565,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>0</v>
@@ -6583,7 +6577,7 @@
         <v>15</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>5</v>
@@ -6591,7 +6585,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>346</v>
@@ -6603,7 +6597,7 @@
         <v>15</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>17</v>
@@ -6611,7 +6605,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>673065</v>
@@ -6625,7 +6619,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>673065</v>
@@ -6639,7 +6633,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>673065</v>
@@ -6653,7 +6647,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>673065</v>
@@ -6667,7 +6661,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>673065</v>
@@ -6681,7 +6675,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>673065</v>

</xml_diff>